<commit_message>
changed some portions of the docs
</commit_message>
<xml_diff>
--- a/Documents/Deliverable drafts_&_templates/Deliverable 4/SixGuys_Deliverable_4_ProductBackLog_6.xlsx
+++ b/Documents/Deliverable drafts_&_templates/Deliverable 4/SixGuys_Deliverable_4_ProductBackLog_6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\Project-Burger\Documents\Deliverable drafts_&amp;_templates\Deliverable 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D504EF-93F3-4056-BD81-B9DFEE954D81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06977A4-4B26-4BCE-B517-E0FC4BBD053C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1350" yWindow="1020" windowWidth="27450" windowHeight="15180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -496,7 +496,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -579,6 +579,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -696,7 +699,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A1:F35" totalsRowShown="0">
   <autoFilter ref="A1:F35" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F35">
-    <sortCondition ref="C2:C35" customList="H,M,L"/>
+    <sortCondition ref="D1:D35"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Sprint Number"/>
@@ -1010,7 +1013,7 @@
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F8" sqref="F8:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -1090,83 +1093,83 @@
       <c r="A4" s="33">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>13</v>
+      <c r="B4" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="9">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="33">
-        <v>1</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>15</v>
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="25" t="s">
-        <v>79</v>
+      <c r="D5" s="20" t="s">
+        <v>8</v>
       </c>
       <c r="E5" s="9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="33">
-        <v>1</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>17</v>
+      <c r="A6" s="34">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="9">
+      <c r="D6" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="9">
         <v>5</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="33">
-        <v>3</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="9">
-        <v>3</v>
-      </c>
       <c r="F7" s="7" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="G7" s="10"/>
     </row>
@@ -1175,40 +1178,40 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="E8" s="9">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="20" t="s">
-        <v>8</v>
+      <c r="D9" s="25" t="s">
+        <v>11</v>
       </c>
       <c r="E9" s="9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="G9" s="10"/>
     </row>
@@ -1216,8 +1219,8 @@
       <c r="A10" s="33">
         <v>3</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>24</v>
+      <c r="B10" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>7</v>
@@ -1226,69 +1229,73 @@
         <v>11</v>
       </c>
       <c r="E10" s="9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="34">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>76</v>
+      <c r="A11" s="33">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="4">
+      <c r="D11" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="9">
+        <v>5</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="33">
         <v>3</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="7"/>
       <c r="B12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>11</v>
       </c>
       <c r="E12" s="9">
         <v>5</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7" t="s">
-        <v>30</v>
+      <c r="A13" s="7">
+        <v>4</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="E13" s="9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G13" s="10"/>
     </row>
@@ -1296,20 +1303,20 @@
       <c r="A14" s="7">
         <v>4</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>32</v>
+      <c r="B14" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E14" s="9">
         <v>5</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="G14" s="10"/>
     </row>
@@ -1318,7 +1325,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>27</v>
@@ -1327,55 +1334,59 @@
         <v>80</v>
       </c>
       <c r="E15" s="9">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="7"/>
+      <c r="A16" s="7">
+        <v>4</v>
+      </c>
       <c r="B16" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>28</v>
+        <v>54</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>11</v>
       </c>
       <c r="E16" s="9">
+        <v>5</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="7">
+        <v>4</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="35">
         <v>2</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="9">
-        <v>2</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>39</v>
+      <c r="F17" s="29" t="s">
+        <v>63</v>
       </c>
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="7"/>
       <c r="B18" s="7" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>27</v>
@@ -1384,17 +1395,17 @@
         <v>28</v>
       </c>
       <c r="E18" s="9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="7"/>
       <c r="B19" s="7" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>27</v>
@@ -1406,14 +1417,14 @@
         <v>5</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="7"/>
       <c r="B20" s="7" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>27</v>
@@ -1422,62 +1433,58 @@
         <v>28</v>
       </c>
       <c r="E20" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="7">
-        <v>4</v>
-      </c>
+      <c r="A21" s="7"/>
       <c r="B21" s="7" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="E21" s="9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="7">
-        <v>4</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>48</v>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="E22" s="9">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="7"/>
       <c r="B23" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>50</v>
+        <v>42</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D23" s="21" t="s">
         <v>28</v>
@@ -1486,17 +1493,17 @@
         <v>5</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="7"/>
       <c r="B24" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>50</v>
+        <v>44</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D24" s="21" t="s">
         <v>28</v>
@@ -1505,35 +1512,33 @@
         <v>1</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="7">
-        <v>4</v>
-      </c>
+      <c r="A25" s="7"/>
       <c r="B25" s="7" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="25" t="s">
-        <v>11</v>
+      <c r="D25" s="21" t="s">
+        <v>28</v>
       </c>
       <c r="E25" s="9">
         <v>5</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="14"/>
       <c r="B26" s="28" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>50</v>
@@ -1542,16 +1547,16 @@
         <v>28</v>
       </c>
       <c r="E26" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="14"/>
-      <c r="B27" s="15" t="s">
-        <v>58</v>
+      <c r="B27" s="28" t="s">
+        <v>56</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>50</v>
@@ -1559,17 +1564,17 @@
       <c r="D27" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="32">
         <v>2</v>
       </c>
-      <c r="F27" s="15" t="s">
-        <v>59</v>
+      <c r="F27" s="28" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="14"/>
       <c r="B28" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>50</v>
@@ -1578,30 +1583,28 @@
         <v>28</v>
       </c>
       <c r="E28" s="17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="14">
-        <v>4</v>
-      </c>
+      <c r="A29" s="14"/>
       <c r="B29" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>50</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="E29" s="17">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:7">

</xml_diff>